<commit_message>
Auswertung_01.xlsx done so far
</commit_message>
<xml_diff>
--- a/docs/Auswertung_01.xlsx
+++ b/docs/Auswertung_01.xlsx
@@ -5,16 +5,20 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Scarlet_Gamma\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FlorianUhde\Documents\Visual Studio 2012\Projects\ADG_Scarlet_Gamma\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12588" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Calculations" sheetId="2" r:id="rId2"/>
+    <sheet name="Diagramme" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>Q1</t>
   </si>
@@ -71,6 +75,39 @@
   <si>
     <t>Test</t>
   </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>2QBox</t>
+  </si>
+  <si>
+    <t>3QBox</t>
+  </si>
+  <si>
+    <t>Whisker-</t>
+  </si>
+  <si>
+    <t>Whisker+</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>BOXPLOT DATA</t>
+  </si>
 </sst>
 </file>
 
@@ -113,12 +150,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -134,6 +176,1518 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Auswertung Fragebogen A</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="minus"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Calculations!$I$14:$R$14</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.25</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.25</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Calculations!$I$2:$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Calculations!$I$11:$R$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Calculations!$I$2:$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Calculations!$I$12:$R$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="plus"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Calculations!$I$15:$R$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.25</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.25</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Calculations!$I$2:$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Q4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Q5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Q6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Q7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Q8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Q9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Q10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Calculations!$I$13:$R$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="-1898026496"/>
+        <c:axId val="-1898028128"/>
+      </c:barChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Calculations!$I$4:$R$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Calculations!$I$16:$R$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1774810320"/>
+        <c:axId val="-1774810864"/>
+      </c:scatterChart>
+      <c:catAx>
+        <c:axId val="-1898026496"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1898028128"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1898028128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1898026496"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1774810864"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1774810320"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1774810320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1774810864"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="O1" t="str">
+            <v>Server Zeit</v>
+          </cell>
+          <cell r="P1" t="str">
+            <v>Transfer Zeit</v>
+          </cell>
+          <cell r="Q1" t="str">
+            <v>Client Zeit</v>
+          </cell>
+          <cell r="R1" t="str">
+            <v>Totale Zeit</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="O10">
+            <v>62</v>
+          </cell>
+          <cell r="P10">
+            <v>16</v>
+          </cell>
+          <cell r="Q10">
+            <v>52</v>
+          </cell>
+          <cell r="R10">
+            <v>156</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="O11">
+            <v>16</v>
+          </cell>
+          <cell r="P11">
+            <v>3</v>
+          </cell>
+          <cell r="Q11">
+            <v>4</v>
+          </cell>
+          <cell r="R11">
+            <v>15</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="O12">
+            <v>0</v>
+          </cell>
+          <cell r="P12">
+            <v>3</v>
+          </cell>
+          <cell r="Q12">
+            <v>4</v>
+          </cell>
+          <cell r="R12">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="O13">
+            <v>16</v>
+          </cell>
+          <cell r="P13">
+            <v>15</v>
+          </cell>
+          <cell r="Q13">
+            <v>27</v>
+          </cell>
+          <cell r="R13">
+            <v>32</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="O14">
+            <v>78</v>
+          </cell>
+          <cell r="P14">
+            <v>28</v>
+          </cell>
+          <cell r="Q14">
+            <v>329</v>
+          </cell>
+          <cell r="R14">
+            <v>312</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -401,16 +1955,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -445,7 +1999,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -477,7 +2031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -517,15 +2071,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F12"/>
+  <dimension ref="B1:R16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R16" activeCellId="1" sqref="I4:R4 I16:R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="18" width="9" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="H1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+    </row>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -538,8 +2112,39 @@
       <c r="F2" t="s">
         <v>13</v>
       </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -559,8 +2164,51 @@
         <f>COUNT(Data!$B:$B)</f>
         <v>2</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="4">
+        <f>COUNT(Data!B:B)</f>
+        <v>2</v>
+      </c>
+      <c r="J3" s="4">
+        <f>COUNT(Data!C:C)</f>
+        <v>2</v>
+      </c>
+      <c r="K3" s="4">
+        <f>COUNT(Data!D:D)</f>
+        <v>2</v>
+      </c>
+      <c r="L3" s="4">
+        <f>COUNT(Data!E:E)</f>
+        <v>2</v>
+      </c>
+      <c r="M3" s="4">
+        <f>COUNT(Data!F:F)</f>
+        <v>2</v>
+      </c>
+      <c r="N3" s="4">
+        <f>COUNT(Data!G:G)</f>
+        <v>2</v>
+      </c>
+      <c r="O3" s="4">
+        <f>COUNT(Data!H:H)</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="4">
+        <f>COUNT(Data!I:I)</f>
+        <v>2</v>
+      </c>
+      <c r="Q3" s="4">
+        <f>COUNT(Data!J:J)</f>
+        <v>2</v>
+      </c>
+      <c r="R3" s="4">
+        <f>COUNT(Data!K:K)</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -580,8 +2228,51 @@
         <f>COUNT(Data!$C:$C)</f>
         <v>2</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="4">
+        <f>AVERAGE(Data!B:B)</f>
+        <v>4</v>
+      </c>
+      <c r="J4" s="4">
+        <f>AVERAGE(Data!C:C)</f>
+        <v>2.5</v>
+      </c>
+      <c r="K4" s="4">
+        <f>AVERAGE(Data!D:D)</f>
+        <v>4</v>
+      </c>
+      <c r="L4" s="4">
+        <f>AVERAGE(Data!E:E)</f>
+        <v>4</v>
+      </c>
+      <c r="M4" s="4">
+        <f>AVERAGE(Data!F:F)</f>
+        <v>4</v>
+      </c>
+      <c r="N4" s="4">
+        <f>AVERAGE(Data!G:G)</f>
+        <v>3</v>
+      </c>
+      <c r="O4" s="4" t="e">
+        <f>AVERAGE(Data!H:H)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P4" s="4">
+        <f>AVERAGE(Data!I:I)</f>
+        <v>4</v>
+      </c>
+      <c r="Q4" s="4">
+        <f>AVERAGE(Data!J:J)</f>
+        <v>4</v>
+      </c>
+      <c r="R4" s="4">
+        <f>AVERAGE(Data!K:K)</f>
+        <v>1.5</v>
+      </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -601,8 +2292,51 @@
         <f>COUNT(Data!$D:$D)</f>
         <v>2</v>
       </c>
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="4">
+        <f>STDEV(Data!B:B)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <f>STDEV(Data!C:C)</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="K5" s="4">
+        <f>STDEV(Data!D:D)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <f>STDEV(Data!E:E)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <f>STDEV(Data!F:F)</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <f>STDEV(Data!G:G)</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="4" t="e">
+        <f>STDEV(Data!H:H)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P5" s="4">
+        <f>STDEV(Data!I:I)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4">
+        <f>STDEV(Data!J:J)</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="4">
+        <f>STDEV(Data!K:K)</f>
+        <v>0.70710678118654757</v>
+      </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -622,8 +2356,51 @@
         <f>COUNT(Data!$E:$E)</f>
         <v>2</v>
       </c>
+      <c r="H6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="4">
+        <f>MIN(Data!B:B)</f>
+        <v>4</v>
+      </c>
+      <c r="J6" s="4">
+        <f>MIN(Data!C:C)</f>
+        <v>2</v>
+      </c>
+      <c r="K6" s="4">
+        <f>MIN(Data!D:D)</f>
+        <v>4</v>
+      </c>
+      <c r="L6" s="4">
+        <f>MIN(Data!E:E)</f>
+        <v>4</v>
+      </c>
+      <c r="M6" s="4">
+        <f>MIN(Data!F:F)</f>
+        <v>4</v>
+      </c>
+      <c r="N6" s="4">
+        <f>MIN(Data!G:G)</f>
+        <v>3</v>
+      </c>
+      <c r="O6" s="4">
+        <f>MIN(Data!H:H)</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="4">
+        <f>MIN(Data!I:I)</f>
+        <v>4</v>
+      </c>
+      <c r="Q6" s="4">
+        <f>MIN(Data!J:J)</f>
+        <v>4</v>
+      </c>
+      <c r="R6" s="4">
+        <f>MIN(Data!K:K)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -643,8 +2420,51 @@
         <f>COUNT(Data!$F:$F)</f>
         <v>2</v>
       </c>
+      <c r="H7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <f>QUARTILE(Data!B:B,1)</f>
+        <v>4</v>
+      </c>
+      <c r="J7" s="4">
+        <f>QUARTILE(Data!C:C,1)</f>
+        <v>2.25</v>
+      </c>
+      <c r="K7" s="4">
+        <f>QUARTILE(Data!D:D,1)</f>
+        <v>4</v>
+      </c>
+      <c r="L7" s="4">
+        <f>QUARTILE(Data!E:E,1)</f>
+        <v>4</v>
+      </c>
+      <c r="M7" s="4">
+        <f>QUARTILE(Data!F:F,1)</f>
+        <v>4</v>
+      </c>
+      <c r="N7" s="4">
+        <f>QUARTILE(Data!G:G,1)</f>
+        <v>3</v>
+      </c>
+      <c r="O7" s="4" t="e">
+        <f>QUARTILE(Data!H:H,1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P7" s="4">
+        <f>QUARTILE(Data!I:I,1)</f>
+        <v>4</v>
+      </c>
+      <c r="Q7" s="4">
+        <f>QUARTILE(Data!J:J,1)</f>
+        <v>4</v>
+      </c>
+      <c r="R7" s="4">
+        <f>QUARTILE(Data!K:K,1)</f>
+        <v>1.25</v>
+      </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -664,8 +2484,51 @@
         <f>COUNT(Data!$G:$G)</f>
         <v>2</v>
       </c>
+      <c r="H8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="4">
+        <f>MEDIAN(Data!B:B)</f>
+        <v>4</v>
+      </c>
+      <c r="J8" s="4">
+        <f>MEDIAN(Data!C:C)</f>
+        <v>2.5</v>
+      </c>
+      <c r="K8" s="4">
+        <f>MEDIAN(Data!D:D)</f>
+        <v>4</v>
+      </c>
+      <c r="L8" s="4">
+        <f>MEDIAN(Data!E:E)</f>
+        <v>4</v>
+      </c>
+      <c r="M8" s="4">
+        <f>MEDIAN(Data!F:F)</f>
+        <v>4</v>
+      </c>
+      <c r="N8" s="4">
+        <f>MEDIAN(Data!G:G)</f>
+        <v>3</v>
+      </c>
+      <c r="O8" s="4" t="e">
+        <f>MEDIAN(Data!H:H)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P8" s="4">
+        <f>MEDIAN(Data!I:I)</f>
+        <v>4</v>
+      </c>
+      <c r="Q8" s="4">
+        <f>MEDIAN(Data!J:J)</f>
+        <v>4</v>
+      </c>
+      <c r="R8" s="4">
+        <f>MEDIAN(Data!K:K)</f>
+        <v>1.5</v>
+      </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -685,8 +2548,51 @@
         <f>COUNT(Data!$H:$H)</f>
         <v>0</v>
       </c>
+      <c r="H9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="4">
+        <f>QUARTILE(Data!B:B,3)</f>
+        <v>4</v>
+      </c>
+      <c r="J9" s="4">
+        <f>QUARTILE(Data!C:C,3)</f>
+        <v>2.75</v>
+      </c>
+      <c r="K9" s="4">
+        <f>QUARTILE(Data!D:D,3)</f>
+        <v>4</v>
+      </c>
+      <c r="L9" s="4">
+        <f>QUARTILE(Data!E:E,3)</f>
+        <v>4</v>
+      </c>
+      <c r="M9" s="4">
+        <f>QUARTILE(Data!F:F,3)</f>
+        <v>4</v>
+      </c>
+      <c r="N9" s="4">
+        <f>QUARTILE(Data!G:G,3)</f>
+        <v>3</v>
+      </c>
+      <c r="O9" s="4" t="e">
+        <f>QUARTILE(Data!H:H,3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P9" s="4">
+        <f>QUARTILE(Data!I:I,3)</f>
+        <v>4</v>
+      </c>
+      <c r="Q9" s="4">
+        <f>QUARTILE(Data!J:J,3)</f>
+        <v>4</v>
+      </c>
+      <c r="R9" s="4">
+        <f>QUARTILE(Data!K:K,3)</f>
+        <v>1.75</v>
+      </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -706,8 +2612,51 @@
         <f>COUNT(Data!$I:$I)</f>
         <v>2</v>
       </c>
+      <c r="H10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="4">
+        <f>MAX(Data!B:B)</f>
+        <v>4</v>
+      </c>
+      <c r="J10" s="4">
+        <f>MAX(Data!C:C)</f>
+        <v>3</v>
+      </c>
+      <c r="K10" s="4">
+        <f>MAX(Data!D:D)</f>
+        <v>4</v>
+      </c>
+      <c r="L10" s="4">
+        <f>MAX(Data!E:E)</f>
+        <v>4</v>
+      </c>
+      <c r="M10" s="4">
+        <f>MAX(Data!F:F)</f>
+        <v>4</v>
+      </c>
+      <c r="N10" s="4">
+        <f>MAX(Data!G:G)</f>
+        <v>3</v>
+      </c>
+      <c r="O10" s="4">
+        <f>MAX(Data!H:H)</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="4">
+        <f>MAX(Data!I:I)</f>
+        <v>4</v>
+      </c>
+      <c r="Q10" s="4">
+        <f>MAX(Data!J:J)</f>
+        <v>4</v>
+      </c>
+      <c r="R10" s="4">
+        <f>MAX(Data!K:K)</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -727,8 +2676,51 @@
         <f>COUNT(Data!$J:$J)</f>
         <v>2</v>
       </c>
+      <c r="H11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="4">
+        <f>I7</f>
+        <v>4</v>
+      </c>
+      <c r="J11" s="4">
+        <f>J7</f>
+        <v>2.25</v>
+      </c>
+      <c r="K11" s="4">
+        <f t="shared" ref="K11:M11" si="0">K7</f>
+        <v>4</v>
+      </c>
+      <c r="L11" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M11" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="N11" s="4">
+        <f>N7</f>
+        <v>3</v>
+      </c>
+      <c r="O11" s="4" t="e">
+        <f>O7</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P11" s="4">
+        <f t="shared" ref="P11:R11" si="1">P7</f>
+        <v>4</v>
+      </c>
+      <c r="Q11" s="4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="R11" s="4">
+        <f t="shared" si="1"/>
+        <v>1.25</v>
+      </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -748,8 +2740,240 @@
         <f>COUNT(Data!$K:$K)</f>
         <v>2</v>
       </c>
+      <c r="H12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" ref="I12:J13" si="2">I8-I7</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="K12" s="4">
+        <f t="shared" ref="K12:O12" si="3">K8-K7</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="4" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P12" s="4">
+        <f t="shared" ref="P12:R12" si="4">P8-P7</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R12" s="4">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="H13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="K13" s="4">
+        <f t="shared" ref="K13:O13" si="5">K9-K8</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="4" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" ref="P13:R13" si="6">P9-P8</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R13" s="4">
+        <f t="shared" si="6"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="H14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="4">
+        <f>I7-I6</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <f>J7-J6</f>
+        <v>0.25</v>
+      </c>
+      <c r="K14" s="4">
+        <f t="shared" ref="K14:M14" si="7">K7-K6</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <f>N7-N6</f>
+        <v>0</v>
+      </c>
+      <c r="O14" s="4" t="e">
+        <f>O7-O6</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P14" s="4">
+        <f t="shared" ref="P14:R14" si="8">P7-P6</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="4">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="H15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="4">
+        <f>I10-I9</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <f>J10-J9</f>
+        <v>0.25</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" ref="K15:M15" si="9">K10-K9</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <f>N10-N9</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="4" t="e">
+        <f>O10-O9</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P15" s="4">
+        <f t="shared" ref="P15:R15" si="10">P10-P9</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="4">
+        <f t="shared" si="10"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="H16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="J16" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K16" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="L16" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="M16" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="N16" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="O16" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="P16" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="R16" s="4">
+        <v>9.5</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H1:R1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor formating to Auswertung_01.xlsx
</commit_message>
<xml_diff>
--- a/docs/Auswertung_01.xlsx
+++ b/docs/Auswertung_01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12588" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12588"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>Q1</t>
   </si>
@@ -107,6 +107,36 @@
   </si>
   <si>
     <t>BOXPLOT DATA</t>
+  </si>
+  <si>
+    <t>Frage 1</t>
+  </si>
+  <si>
+    <t>Frage 2</t>
+  </si>
+  <si>
+    <t>Frage 3</t>
+  </si>
+  <si>
+    <t>Frage 4</t>
+  </si>
+  <si>
+    <t>Frage 5</t>
+  </si>
+  <si>
+    <t>Frage 6</t>
+  </si>
+  <si>
+    <t>Frage 7</t>
+  </si>
+  <si>
+    <t>Frage 8</t>
+  </si>
+  <si>
+    <t>Frage 9</t>
+  </si>
+  <si>
+    <t>Frage 10</t>
   </si>
 </sst>
 </file>
@@ -338,34 +368,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Q1</c:v>
+                  <c:v>Frage 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Q2</c:v>
+                  <c:v>Frage 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Q3</c:v>
+                  <c:v>Frage 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Q4</c:v>
+                  <c:v>Frage 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Q5</c:v>
+                  <c:v>Frage 5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Q6</c:v>
+                  <c:v>Frage 6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Q7</c:v>
+                  <c:v>Frage 7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Q8</c:v>
+                  <c:v>Frage 8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Q9</c:v>
+                  <c:v>Frage 9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Q10</c:v>
+                  <c:v>Frage 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -432,34 +462,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Q1</c:v>
+                  <c:v>Frage 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Q2</c:v>
+                  <c:v>Frage 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Q3</c:v>
+                  <c:v>Frage 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Q4</c:v>
+                  <c:v>Frage 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Q5</c:v>
+                  <c:v>Frage 5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Q6</c:v>
+                  <c:v>Frage 6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Q7</c:v>
+                  <c:v>Frage 7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Q8</c:v>
+                  <c:v>Frage 8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Q9</c:v>
+                  <c:v>Frage 9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Q10</c:v>
+                  <c:v>Frage 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -592,34 +622,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Q1</c:v>
+                  <c:v>Frage 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Q2</c:v>
+                  <c:v>Frage 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Q3</c:v>
+                  <c:v>Frage 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Q4</c:v>
+                  <c:v>Frage 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Q5</c:v>
+                  <c:v>Frage 5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Q6</c:v>
+                  <c:v>Frage 6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Q7</c:v>
+                  <c:v>Frage 7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Q8</c:v>
+                  <c:v>Frage 8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Q9</c:v>
+                  <c:v>Frage 9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Q10</c:v>
+                  <c:v>Frage 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1955,8 +1985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2074,7 +2104,7 @@
   <dimension ref="B1:R16"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R16" activeCellId="1" sqref="I4:R4 I16:R16"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2114,34 +2144,34 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
@@ -2967,7 +2997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated evaluation with some more data
</commit_message>
<xml_diff>
--- a/docs/Auswertung_01.xlsx
+++ b/docs/Auswertung_01.xlsx
@@ -1,25 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FlorianUhde\Documents\Visual Studio 2012\Projects\ADG_Scarlet_Gamma\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12588"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Calculations" sheetId="2" r:id="rId2"/>
     <sheet name="Diagramme" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>Q1</t>
   </si>
@@ -137,13 +129,34 @@
   </si>
   <si>
     <t>Frage 10</t>
+  </si>
+  <si>
+    <t>Zeiten in s</t>
+  </si>
+  <si>
+    <t>Karte erstellen</t>
+  </si>
+  <si>
+    <t>3 Räume</t>
+  </si>
+  <si>
+    <t>Mob</t>
+  </si>
+  <si>
+    <t>Interaktionsgegenstand</t>
+  </si>
+  <si>
+    <t>Gegner setzen</t>
+  </si>
+  <si>
+    <t>Schatztruhe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +171,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -180,20 +200,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -211,7 +235,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -257,26 +281,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -319,7 +323,7 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.25</c:v>
+                    <c:v>1.5</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0</c:v>
@@ -337,13 +341,13 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0</c:v>
+                    <c:v>1</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0</c:v>
+                    <c:v>1</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0.25</c:v>
+                    <c:v>1</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -410,7 +414,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.25</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
@@ -419,22 +423,22 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.25</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -504,7 +508,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -513,13 +517,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -528,7 +532,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.25</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -564,7 +568,7 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.25</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0</c:v>
@@ -588,7 +592,7 @@
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0.25</c:v>
+                    <c:v>0.5</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -664,7 +668,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -676,7 +680,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -685,10 +689,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.25</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -704,8 +708,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1898026496"/>
-        <c:axId val="-1898028128"/>
+        <c:axId val="147672448"/>
+        <c:axId val="147469824"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -745,7 +749,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
@@ -754,22 +758,22 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>3.5714285714285716</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>3.4285714285714284</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>3.8571428571428572</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>3.2857142857142856</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.5</c:v>
+                  <c:v>2.7142857142857144</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -823,11 +827,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1774810320"/>
-        <c:axId val="-1774810864"/>
+        <c:axId val="147473152"/>
+        <c:axId val="147471360"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="-1898026496"/>
+        <c:axId val="147672448"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -870,7 +874,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1898028128"/>
+        <c:crossAx val="147469824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -878,7 +882,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1898028128"/>
+        <c:axId val="147469824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -930,13 +934,13 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1898026496"/>
+        <c:crossAx val="147672448"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1774810864"/>
+        <c:axId val="147471360"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -973,22 +977,23 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1774810320"/>
+        <c:crossAx val="147473152"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1774810320"/>
+        <c:axId val="147473152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1774810864"/>
+        <c:crossAx val="147471360"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1618,108 +1623,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Sheet3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="O1" t="str">
-            <v>Server Zeit</v>
-          </cell>
-          <cell r="P1" t="str">
-            <v>Transfer Zeit</v>
-          </cell>
-          <cell r="Q1" t="str">
-            <v>Client Zeit</v>
-          </cell>
-          <cell r="R1" t="str">
-            <v>Totale Zeit</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="O10">
-            <v>62</v>
-          </cell>
-          <cell r="P10">
-            <v>16</v>
-          </cell>
-          <cell r="Q10">
-            <v>52</v>
-          </cell>
-          <cell r="R10">
-            <v>156</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="O11">
-            <v>16</v>
-          </cell>
-          <cell r="P11">
-            <v>3</v>
-          </cell>
-          <cell r="Q11">
-            <v>4</v>
-          </cell>
-          <cell r="R11">
-            <v>15</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="O12">
-            <v>0</v>
-          </cell>
-          <cell r="P12">
-            <v>3</v>
-          </cell>
-          <cell r="Q12">
-            <v>4</v>
-          </cell>
-          <cell r="R12">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="O13">
-            <v>16</v>
-          </cell>
-          <cell r="P13">
-            <v>15</v>
-          </cell>
-          <cell r="Q13">
-            <v>27</v>
-          </cell>
-          <cell r="R13">
-            <v>32</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="O14">
-            <v>78</v>
-          </cell>
-          <cell r="P14">
-            <v>28</v>
-          </cell>
-          <cell r="Q14">
-            <v>329</v>
-          </cell>
-          <cell r="R14">
-            <v>312</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1975,7 +1878,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1983,54 +1886,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="O1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2">
@@ -2061,8 +1985,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3">
@@ -2091,6 +2015,235 @@
       </c>
       <c r="K3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>30</v>
+      </c>
+      <c r="Q4">
+        <v>60</v>
+      </c>
+      <c r="R4">
+        <v>130</v>
+      </c>
+      <c r="S4">
+        <v>100</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>30</v>
+      </c>
+      <c r="Q5">
+        <v>60</v>
+      </c>
+      <c r="R5">
+        <v>240</v>
+      </c>
+      <c r="S5">
+        <v>30</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <v>120</v>
+      </c>
+      <c r="Q6">
+        <v>180</v>
+      </c>
+      <c r="R6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="P7">
+        <v>30</v>
+      </c>
+      <c r="Q7">
+        <v>180</v>
+      </c>
+      <c r="R7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2107,27 +2260,27 @@
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="18" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
@@ -2192,50 +2345,50 @@
       </c>
       <c r="F3">
         <f>COUNT(Data!$B:$B)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <f>COUNT(Data!B:B)</f>
-        <v>2</v>
-      </c>
-      <c r="J3" s="4">
+        <v>7</v>
+      </c>
+      <c r="J3" s="3">
         <f>COUNT(Data!C:C)</f>
-        <v>2</v>
-      </c>
-      <c r="K3" s="4">
+        <v>7</v>
+      </c>
+      <c r="K3" s="3">
         <f>COUNT(Data!D:D)</f>
-        <v>2</v>
-      </c>
-      <c r="L3" s="4">
+        <v>7</v>
+      </c>
+      <c r="L3" s="3">
         <f>COUNT(Data!E:E)</f>
-        <v>2</v>
-      </c>
-      <c r="M3" s="4">
+        <v>7</v>
+      </c>
+      <c r="M3" s="3">
         <f>COUNT(Data!F:F)</f>
-        <v>2</v>
-      </c>
-      <c r="N3" s="4">
+        <v>7</v>
+      </c>
+      <c r="N3" s="3">
         <f>COUNT(Data!G:G)</f>
-        <v>2</v>
-      </c>
-      <c r="O3" s="4">
+        <v>7</v>
+      </c>
+      <c r="O3" s="3">
         <f>COUNT(Data!H:H)</f>
-        <v>0</v>
-      </c>
-      <c r="P3" s="4">
+        <v>5</v>
+      </c>
+      <c r="P3" s="3">
         <f>COUNT(Data!I:I)</f>
-        <v>2</v>
-      </c>
-      <c r="Q3" s="4">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="3">
         <f>COUNT(Data!J:J)</f>
-        <v>2</v>
-      </c>
-      <c r="R3" s="4">
+        <v>7</v>
+      </c>
+      <c r="R3" s="3">
         <f>COUNT(Data!K:K)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
@@ -2244,62 +2397,62 @@
       </c>
       <c r="C4">
         <f>MAX(Data!$C:$C)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <f>MIN(Data!$C:$C)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <f>AVERAGE(Data!$C:$C)</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <f>COUNT(Data!$C:$C)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <f>AVERAGE(Data!B:B)</f>
         <v>4</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <f>AVERAGE(Data!C:C)</f>
-        <v>2.5</v>
-      </c>
-      <c r="K4" s="4">
+        <v>3</v>
+      </c>
+      <c r="K4" s="3">
         <f>AVERAGE(Data!D:D)</f>
         <v>4</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <f>AVERAGE(Data!E:E)</f>
         <v>4</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="3">
         <f>AVERAGE(Data!F:F)</f>
-        <v>4</v>
-      </c>
-      <c r="N4" s="4">
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="N4" s="3">
         <f>AVERAGE(Data!G:G)</f>
-        <v>3</v>
-      </c>
-      <c r="O4" s="4" t="e">
+        <v>3.4285714285714284</v>
+      </c>
+      <c r="O4" s="3">
         <f>AVERAGE(Data!H:H)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P4" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="P4" s="3">
         <f>AVERAGE(Data!I:I)</f>
-        <v>4</v>
-      </c>
-      <c r="Q4" s="4">
+        <v>3.8571428571428572</v>
+      </c>
+      <c r="Q4" s="3">
         <f>AVERAGE(Data!J:J)</f>
-        <v>4</v>
-      </c>
-      <c r="R4" s="4">
+        <v>3.2857142857142856</v>
+      </c>
+      <c r="R4" s="3">
         <f>AVERAGE(Data!K:K)</f>
-        <v>1.5</v>
+        <v>2.7142857142857144</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
@@ -2320,50 +2473,50 @@
       </c>
       <c r="F5">
         <f>COUNT(Data!$D:$D)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <f>STDEV(Data!B:B)</f>
         <v>0</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <f>STDEV(Data!C:C)</f>
-        <v>0.70710678118654757</v>
-      </c>
-      <c r="K5" s="4">
+        <v>1.1547005383792515</v>
+      </c>
+      <c r="K5" s="3">
         <f>STDEV(Data!D:D)</f>
         <v>0</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <f>STDEV(Data!E:E)</f>
         <v>0</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="3">
         <f>STDEV(Data!F:F)</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="4">
+        <v>0.53452248382484779</v>
+      </c>
+      <c r="N5" s="3">
         <f>STDEV(Data!G:G)</f>
-        <v>0</v>
-      </c>
-      <c r="O5" s="4" t="e">
+        <v>0.53452248382484779</v>
+      </c>
+      <c r="O5" s="3">
         <f>STDEV(Data!H:H)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P5" s="4">
+        <v>0.54772255750516674</v>
+      </c>
+      <c r="P5" s="3">
         <f>STDEV(Data!I:I)</f>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="4">
+        <v>0.37796447300922725</v>
+      </c>
+      <c r="Q5" s="3">
         <f>STDEV(Data!J:J)</f>
-        <v>0</v>
-      </c>
-      <c r="R5" s="4">
+        <v>0.75592894601845462</v>
+      </c>
+      <c r="R5" s="3">
         <f>STDEV(Data!K:K)</f>
-        <v>0.70710678118654757</v>
+        <v>1.1126972805283737</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
@@ -2384,48 +2537,48 @@
       </c>
       <c r="F6">
         <f>COUNT(Data!$E:$E)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <f>MIN(Data!B:B)</f>
         <v>4</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <f>MIN(Data!C:C)</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="3">
+        <f>MIN(Data!D:D)</f>
+        <v>4</v>
+      </c>
+      <c r="L6" s="3">
+        <f>MIN(Data!E:E)</f>
+        <v>4</v>
+      </c>
+      <c r="M6" s="3">
+        <f>MIN(Data!F:F)</f>
+        <v>3</v>
+      </c>
+      <c r="N6" s="3">
+        <f>MIN(Data!G:G)</f>
+        <v>3</v>
+      </c>
+      <c r="O6" s="3">
+        <f>MIN(Data!H:H)</f>
+        <v>3</v>
+      </c>
+      <c r="P6" s="3">
+        <f>MIN(Data!I:I)</f>
+        <v>3</v>
+      </c>
+      <c r="Q6" s="3">
+        <f>MIN(Data!J:J)</f>
         <v>2</v>
       </c>
-      <c r="K6" s="4">
-        <f>MIN(Data!D:D)</f>
-        <v>4</v>
-      </c>
-      <c r="L6" s="4">
-        <f>MIN(Data!E:E)</f>
-        <v>4</v>
-      </c>
-      <c r="M6" s="4">
-        <f>MIN(Data!F:F)</f>
-        <v>4</v>
-      </c>
-      <c r="N6" s="4">
-        <f>MIN(Data!G:G)</f>
-        <v>3</v>
-      </c>
-      <c r="O6" s="4">
-        <f>MIN(Data!H:H)</f>
-        <v>0</v>
-      </c>
-      <c r="P6" s="4">
-        <f>MIN(Data!I:I)</f>
-        <v>4</v>
-      </c>
-      <c r="Q6" s="4">
-        <f>MIN(Data!J:J)</f>
-        <v>4</v>
-      </c>
-      <c r="R6" s="4">
+      <c r="R6" s="3">
         <f>MIN(Data!K:K)</f>
         <v>1</v>
       </c>
@@ -2440,58 +2593,58 @@
       </c>
       <c r="D7">
         <f>MIN(Data!$F:$F)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <f>AVERAGE(Data!$F:$F)</f>
-        <v>4</v>
+        <v>3.5714285714285716</v>
       </c>
       <c r="F7">
         <f>COUNT(Data!$F:$F)</f>
+        <v>7</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <f>QUARTILE(Data!B:B,1)</f>
+        <v>4</v>
+      </c>
+      <c r="J7" s="3">
+        <f>QUARTILE(Data!C:C,1)</f>
+        <v>2.5</v>
+      </c>
+      <c r="K7" s="3">
+        <f>QUARTILE(Data!D:D,1)</f>
+        <v>4</v>
+      </c>
+      <c r="L7" s="3">
+        <f>QUARTILE(Data!E:E,1)</f>
+        <v>4</v>
+      </c>
+      <c r="M7" s="3">
+        <f>QUARTILE(Data!F:F,1)</f>
+        <v>3</v>
+      </c>
+      <c r="N7" s="3">
+        <f>QUARTILE(Data!G:G,1)</f>
+        <v>3</v>
+      </c>
+      <c r="O7" s="3">
+        <f>QUARTILE(Data!H:H,1)</f>
+        <v>3</v>
+      </c>
+      <c r="P7" s="3">
+        <f>QUARTILE(Data!I:I,1)</f>
+        <v>4</v>
+      </c>
+      <c r="Q7" s="3">
+        <f>QUARTILE(Data!J:J,1)</f>
+        <v>3</v>
+      </c>
+      <c r="R7" s="3">
+        <f>QUARTILE(Data!K:K,1)</f>
         <v>2</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
-        <f>QUARTILE(Data!B:B,1)</f>
-        <v>4</v>
-      </c>
-      <c r="J7" s="4">
-        <f>QUARTILE(Data!C:C,1)</f>
-        <v>2.25</v>
-      </c>
-      <c r="K7" s="4">
-        <f>QUARTILE(Data!D:D,1)</f>
-        <v>4</v>
-      </c>
-      <c r="L7" s="4">
-        <f>QUARTILE(Data!E:E,1)</f>
-        <v>4</v>
-      </c>
-      <c r="M7" s="4">
-        <f>QUARTILE(Data!F:F,1)</f>
-        <v>4</v>
-      </c>
-      <c r="N7" s="4">
-        <f>QUARTILE(Data!G:G,1)</f>
-        <v>3</v>
-      </c>
-      <c r="O7" s="4" t="e">
-        <f>QUARTILE(Data!H:H,1)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="P7" s="4">
-        <f>QUARTILE(Data!I:I,1)</f>
-        <v>4</v>
-      </c>
-      <c r="Q7" s="4">
-        <f>QUARTILE(Data!J:J,1)</f>
-        <v>4</v>
-      </c>
-      <c r="R7" s="4">
-        <f>QUARTILE(Data!K:K,1)</f>
-        <v>1.25</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
@@ -2500,7 +2653,7 @@
       </c>
       <c r="C8">
         <f>MAX(Data!$G:$G)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <f>MIN(Data!$G:$G)</f>
@@ -2508,54 +2661,54 @@
       </c>
       <c r="E8">
         <f>AVERAGE(Data!$G:$G)</f>
-        <v>3</v>
+        <v>3.4285714285714284</v>
       </c>
       <c r="F8">
         <f>COUNT(Data!$G:$G)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <f>MEDIAN(Data!B:B)</f>
         <v>4</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="3">
         <f>MEDIAN(Data!C:C)</f>
-        <v>2.5</v>
-      </c>
-      <c r="K8" s="4">
+        <v>3</v>
+      </c>
+      <c r="K8" s="3">
         <f>MEDIAN(Data!D:D)</f>
         <v>4</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="3">
         <f>MEDIAN(Data!E:E)</f>
         <v>4</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="3">
         <f>MEDIAN(Data!F:F)</f>
         <v>4</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8" s="3">
         <f>MEDIAN(Data!G:G)</f>
         <v>3</v>
       </c>
-      <c r="O8" s="4" t="e">
+      <c r="O8" s="3">
         <f>MEDIAN(Data!H:H)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="P8" s="4">
+        <v>4</v>
+      </c>
+      <c r="P8" s="3">
         <f>MEDIAN(Data!I:I)</f>
         <v>4</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="Q8" s="3">
         <f>MEDIAN(Data!J:J)</f>
-        <v>4</v>
-      </c>
-      <c r="R8" s="4">
+        <v>3</v>
+      </c>
+      <c r="R8" s="3">
         <f>MEDIAN(Data!K:K)</f>
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
@@ -2564,62 +2717,62 @@
       </c>
       <c r="C9">
         <f>MAX(Data!$H:$H)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <f>MIN(Data!$H:$H)</f>
-        <v>0</v>
-      </c>
-      <c r="E9" t="e">
+        <v>3</v>
+      </c>
+      <c r="E9">
         <f>AVERAGE(Data!$H:$H)</f>
-        <v>#DIV/0!</v>
+        <v>3.6</v>
       </c>
       <c r="F9">
         <f>COUNT(Data!$H:$H)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <f>QUARTILE(Data!B:B,3)</f>
         <v>4</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="3">
         <f>QUARTILE(Data!C:C,3)</f>
-        <v>2.75</v>
-      </c>
-      <c r="K9" s="4">
+        <v>4</v>
+      </c>
+      <c r="K9" s="3">
         <f>QUARTILE(Data!D:D,3)</f>
         <v>4</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="3">
         <f>QUARTILE(Data!E:E,3)</f>
         <v>4</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="3">
         <f>QUARTILE(Data!F:F,3)</f>
         <v>4</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="3">
         <f>QUARTILE(Data!G:G,3)</f>
-        <v>3</v>
-      </c>
-      <c r="O9" s="4" t="e">
+        <v>4</v>
+      </c>
+      <c r="O9" s="3">
         <f>QUARTILE(Data!H:H,3)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="P9" s="4">
+        <v>4</v>
+      </c>
+      <c r="P9" s="3">
         <f>QUARTILE(Data!I:I,3)</f>
         <v>4</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q9" s="3">
         <f>QUARTILE(Data!J:J,3)</f>
         <v>4</v>
       </c>
-      <c r="R9" s="4">
+      <c r="R9" s="3">
         <f>QUARTILE(Data!K:K,3)</f>
-        <v>1.75</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
@@ -2632,58 +2785,58 @@
       </c>
       <c r="D10">
         <f>MIN(Data!$I:$I)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <f>AVERAGE(Data!$I:$I)</f>
-        <v>4</v>
+        <v>3.8571428571428572</v>
       </c>
       <c r="F10">
         <f>COUNT(Data!$I:$I)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <f>MAX(Data!B:B)</f>
         <v>4</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="3">
         <f>MAX(Data!C:C)</f>
-        <v>3</v>
-      </c>
-      <c r="K10" s="4">
+        <v>4</v>
+      </c>
+      <c r="K10" s="3">
         <f>MAX(Data!D:D)</f>
         <v>4</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="3">
         <f>MAX(Data!E:E)</f>
         <v>4</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="3">
         <f>MAX(Data!F:F)</f>
         <v>4</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10" s="3">
         <f>MAX(Data!G:G)</f>
-        <v>3</v>
-      </c>
-      <c r="O10" s="4">
+        <v>4</v>
+      </c>
+      <c r="O10" s="3">
         <f>MAX(Data!H:H)</f>
-        <v>0</v>
-      </c>
-      <c r="P10" s="4">
+        <v>4</v>
+      </c>
+      <c r="P10" s="3">
         <f>MAX(Data!I:I)</f>
         <v>4</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="Q10" s="3">
         <f>MAX(Data!J:J)</f>
         <v>4</v>
       </c>
-      <c r="R10" s="4">
+      <c r="R10" s="3">
         <f>MAX(Data!K:K)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
@@ -2696,58 +2849,58 @@
       </c>
       <c r="D11">
         <f>MIN(Data!$J:$J)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E11">
         <f>AVERAGE(Data!$J:$J)</f>
-        <v>4</v>
+        <v>3.2857142857142856</v>
       </c>
       <c r="F11">
         <f>COUNT(Data!$J:$J)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <f>I7</f>
         <v>4</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="3">
         <f>J7</f>
-        <v>2.25</v>
-      </c>
-      <c r="K11" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="K11" s="3">
         <f t="shared" ref="K11:M11" si="0">K7</f>
         <v>4</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="3">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="N11" s="4">
+        <v>3</v>
+      </c>
+      <c r="N11" s="3">
         <f>N7</f>
         <v>3</v>
       </c>
-      <c r="O11" s="4" t="e">
+      <c r="O11" s="3">
         <f>O7</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="P11" s="4">
+        <v>3</v>
+      </c>
+      <c r="P11" s="3">
         <f t="shared" ref="P11:R11" si="1">P7</f>
         <v>4</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="Q11" s="3">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="R11" s="4">
+        <v>3</v>
+      </c>
+      <c r="R11" s="3">
         <f t="shared" si="1"/>
-        <v>1.25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
@@ -2756,7 +2909,7 @@
       </c>
       <c r="C12">
         <f>MAX(Data!$K:$K)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <f>MIN(Data!$K:$K)</f>
@@ -2764,223 +2917,223 @@
       </c>
       <c r="E12">
         <f>AVERAGE(Data!$K:$K)</f>
-        <v>1.5</v>
+        <v>2.7142857142857144</v>
       </c>
       <c r="F12">
         <f>COUNT(Data!$K:$K)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <f t="shared" ref="I12:J13" si="2">I8-I7</f>
         <v>0</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="3">
         <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="K12" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K12" s="3">
         <f t="shared" ref="K12:O12" si="3">K8-K7</f>
         <v>0</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O12" s="4" t="e">
+      <c r="O12" s="3">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="P12" s="4">
+        <v>1</v>
+      </c>
+      <c r="P12" s="3">
         <f t="shared" ref="P12:R12" si="4">P8-P7</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="Q12" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="R12" s="4">
+      <c r="R12" s="3">
         <f t="shared" si="4"/>
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="H13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="3">
         <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="K13" s="4">
+        <v>1</v>
+      </c>
+      <c r="K13" s="3">
         <f t="shared" ref="K13:O13" si="5">K9-K8</f>
         <v>0</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="4" t="e">
+        <v>1</v>
+      </c>
+      <c r="O13" s="3">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="P13" s="4">
+        <v>0</v>
+      </c>
+      <c r="P13" s="3">
         <f t="shared" ref="P13:R13" si="6">P9-P8</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="Q13" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R13" s="4">
+        <v>1</v>
+      </c>
+      <c r="R13" s="3">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="H14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <f>I7-I6</f>
         <v>0</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="3">
         <f>J7-J6</f>
-        <v>0.25</v>
-      </c>
-      <c r="K14" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K14" s="3">
         <f t="shared" ref="K14:M14" si="7">K7-K6</f>
         <v>0</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="3">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14" s="3">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="N14" s="4">
+      <c r="N14" s="3">
         <f>N7-N6</f>
         <v>0</v>
       </c>
-      <c r="O14" s="4" t="e">
+      <c r="O14" s="3">
         <f>O7-O6</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="P14" s="4">
+        <v>0</v>
+      </c>
+      <c r="P14" s="3">
         <f t="shared" ref="P14:R14" si="8">P7-P6</f>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="3">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="R14" s="4">
+        <v>1</v>
+      </c>
+      <c r="R14" s="3">
         <f t="shared" si="8"/>
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="H15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <f>I10-I9</f>
         <v>0</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="3">
         <f>J10-J9</f>
-        <v>0.25</v>
-      </c>
-      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3">
         <f t="shared" ref="K15:M15" si="9">K10-K9</f>
         <v>0</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="3">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15" s="3">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="N15" s="4">
+      <c r="N15" s="3">
         <f>N10-N9</f>
         <v>0</v>
       </c>
-      <c r="O15" s="4" t="e">
+      <c r="O15" s="3">
         <f>O10-O9</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="P15" s="4">
+        <v>0</v>
+      </c>
+      <c r="P15" s="3">
         <f t="shared" ref="P15:R15" si="10">P10-P9</f>
         <v>0</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="Q15" s="3">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="R15" s="4">
+      <c r="R15" s="3">
         <f t="shared" si="10"/>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="3">
         <v>0.5</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="3">
         <v>1.5</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="3">
         <v>2.5</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="3">
         <v>3.5</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16" s="3">
         <v>4.5</v>
       </c>
-      <c r="N16" s="4">
+      <c r="N16" s="3">
         <v>5.5</v>
       </c>
-      <c r="O16" s="4">
+      <c r="O16" s="3">
         <v>6.5</v>
       </c>
-      <c r="P16" s="4">
+      <c r="P16" s="3">
         <v>7.5</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="Q16" s="3">
         <v>8.5</v>
       </c>
-      <c r="R16" s="4">
+      <c r="R16" s="3">
         <v>9.5</v>
       </c>
     </row>
@@ -2997,11 +3150,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
extended excel sheet to better show quartils with some questions
</commit_message>
<xml_diff>
--- a/docs/Auswertung_01.xlsx
+++ b/docs/Auswertung_01.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FlorianUhde\Documents\Visual Studio 2012\Projects\ADG_Scarlet_Gamma\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12588" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Calculations" sheetId="2" r:id="rId2"/>
     <sheet name="Diagramme" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>Q1</t>
   </si>
@@ -150,6 +155,9 @@
   </si>
   <si>
     <t>Schatztruhe</t>
+  </si>
+  <si>
+    <t>EnlargeCell</t>
   </si>
 </sst>
 </file>
@@ -208,16 +216,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -235,7 +243,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -281,6 +289,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -411,16 +439,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>3.98</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>3.98</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>3.98</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3</c:v>
@@ -432,7 +460,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>3.98</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>3</c:v>
@@ -505,16 +533,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -526,7 +554,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -665,16 +693,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -686,7 +714,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
@@ -708,8 +736,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="147672448"/>
-        <c:axId val="147469824"/>
+        <c:axId val="-410372464"/>
+        <c:axId val="-410370288"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -827,11 +855,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="147473152"/>
-        <c:axId val="147471360"/>
+        <c:axId val="-343984144"/>
+        <c:axId val="-410381712"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="147672448"/>
+        <c:axId val="-410372464"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -874,7 +902,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147469824"/>
+        <c:crossAx val="-410370288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -882,10 +910,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147469824"/>
+        <c:axId val="-410370288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4"/>
+          <c:max val="4.2"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -934,13 +963,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147672448"/>
+        <c:crossAx val="-410372464"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
+        <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147471360"/>
+        <c:axId val="-410381712"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -977,12 +1007,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147473152"/>
+        <c:crossAx val="-343984144"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147473152"/>
+        <c:axId val="-343984144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -992,7 +1022,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147471360"/>
+        <c:crossAx val="-410381712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1878,7 +1908,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1888,47 +1918,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="7" t="s">
+      <c r="E1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="O1" t="s">
@@ -1953,8 +1983,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2">
@@ -1985,8 +2015,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3">
@@ -2017,8 +2047,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4">
@@ -2070,8 +2100,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5">
@@ -2123,8 +2153,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6">
@@ -2167,8 +2197,8 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7">
@@ -2211,8 +2241,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8">
@@ -2254,33 +2284,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R16"/>
+  <dimension ref="B1:R18"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="K11" sqref="I11:K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="18" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
@@ -2863,36 +2893,36 @@
         <v>19</v>
       </c>
       <c r="I11" s="3">
-        <f>I7</f>
-        <v>4</v>
+        <f t="shared" ref="I11:J11" si="0">IF(I18,I7-0.02,I7)</f>
+        <v>3.98</v>
       </c>
       <c r="J11" s="3">
-        <f>J7</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="K11" s="3">
-        <f t="shared" ref="K11:M11" si="0">K7</f>
-        <v>4</v>
+        <f>IF(K18,K7-0.02,K7)</f>
+        <v>3.98</v>
       </c>
       <c r="L11" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" ref="L11:R11" si="1">IF(L18,L7-0.02,L7)</f>
+        <v>3.98</v>
       </c>
       <c r="M11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="N11" s="3">
-        <f>N7</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="O11" s="3">
-        <f>O7</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="P11" s="3">
-        <f t="shared" ref="P11:R11" si="1">P7</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>3.98</v>
       </c>
       <c r="Q11" s="3">
         <f t="shared" si="1"/>
@@ -2927,20 +2957,20 @@
         <v>20</v>
       </c>
       <c r="I12" s="3">
-        <f t="shared" ref="I12:J13" si="2">I8-I7</f>
-        <v>0</v>
+        <f t="shared" ref="I12:J12" si="2">IF(I18,I8-I7+0.02,I8-I7)</f>
+        <v>0.02</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="K12" s="3">
-        <f t="shared" ref="K12:O12" si="3">K8-K7</f>
-        <v>0</v>
+        <f>IF(K18,K8-K7+0.02,K8-K7)</f>
+        <v>0.02</v>
       </c>
       <c r="L12" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="L12:R12" si="3">IF(L18,L8-L7+0.02,L8-L7)</f>
+        <v>0.02</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="3"/>
@@ -2955,15 +2985,15 @@
         <v>1</v>
       </c>
       <c r="P12" s="3">
-        <f t="shared" ref="P12:R12" si="4">P8-P7</f>
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+      <c r="Q12" s="3">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q12" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="R12" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2972,20 +3002,20 @@
         <v>21</v>
       </c>
       <c r="I13" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="I13:J13" si="4">IF(I18,I9-I8+0.02,I9-I8)</f>
+        <v>0.02</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K13" s="3">
-        <f t="shared" ref="K13:O13" si="5">K9-K8</f>
-        <v>0</v>
+        <f>IF(K18,K9-K8+0.02,K9-K8)</f>
+        <v>0.02</v>
       </c>
       <c r="L13" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" ref="L13:R13" si="5">IF(L18,L9-L8+0.02,L9-L8)</f>
+        <v>0.02</v>
       </c>
       <c r="M13" s="3">
         <f t="shared" si="5"/>
@@ -3000,15 +3030,15 @@
         <v>0</v>
       </c>
       <c r="P13" s="3">
-        <f t="shared" ref="P13:R13" si="6">P9-P8</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0.02</v>
       </c>
       <c r="Q13" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R13" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3025,15 +3055,15 @@
         <v>1.5</v>
       </c>
       <c r="K14" s="3">
-        <f t="shared" ref="K14:M14" si="7">K7-K6</f>
+        <f t="shared" ref="K14:M14" si="6">K7-K6</f>
         <v>0</v>
       </c>
       <c r="L14" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M14" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N14" s="3">
@@ -3045,15 +3075,15 @@
         <v>0</v>
       </c>
       <c r="P14" s="3">
-        <f t="shared" ref="P14:R14" si="8">P7-P6</f>
+        <f t="shared" ref="P14:R14" si="7">P7-P6</f>
         <v>1</v>
       </c>
       <c r="Q14" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="R14" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3070,15 +3100,15 @@
         <v>0</v>
       </c>
       <c r="K15" s="3">
-        <f t="shared" ref="K15:M15" si="9">K10-K9</f>
+        <f t="shared" ref="K15:M15" si="8">K10-K9</f>
         <v>0</v>
       </c>
       <c r="L15" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M15" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N15" s="3">
@@ -3090,15 +3120,15 @@
         <v>0</v>
       </c>
       <c r="P15" s="3">
-        <f t="shared" ref="P15:R15" si="10">P10-P9</f>
+        <f t="shared" ref="P15:R15" si="9">P10-P9</f>
         <v>0</v>
       </c>
       <c r="Q15" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R15" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
     </row>
@@ -3135,6 +3165,51 @@
       </c>
       <c r="R16" s="3">
         <v>9.5</v>
+      </c>
+    </row>
+    <row r="18" spans="8:18" x14ac:dyDescent="0.3">
+      <c r="H18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" t="b">
+        <f>IF(I8-I7=I9-I8,IF(I8-I7=0,TRUE),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J18" t="b">
+        <f>IF(J8-J7=J9-J8,IF(J8-J7=0,TRUE),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="K18" t="b">
+        <f>IF(K8-K7=K9-K8,IF(K8-K7=0,TRUE),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="L18" t="b">
+        <f t="shared" ref="L18:R18" si="10">IF(L8-L7=L9-L8,IF(L8-L7=0,TRUE),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="M18" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N18" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="O18" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P18" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="Q18" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="R18" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3150,11 +3225,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>